<commit_message>
Removing headers, adding to guide
</commit_message>
<xml_diff>
--- a/fhir-resource-tooling/src/test/resources/2.16.840.1.113762.1.4.1114.7-Comments.xlsx
+++ b/fhir-resource-tooling/src/test/resources/2.16.840.1.113762.1.4.1114.7-Comments.xlsx
@@ -5,21 +5,32 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mshelley/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mshelley/Documents/weirdStuff/quality-measure-and-cohort-service/fhir-resource-tooling/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C2483A20-B597-FF46-AB1B-7C69A77EB9BE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A48E49A1-F61B-BC4C-BBD6-D72BF0B4C6E5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="480" windowWidth="33600" windowHeight="20540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Value Set Info" sheetId="1" r:id="rId1"/>
     <sheet name="Expansion List" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Expansion List'!$A$13:$F$13</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Expansion List'!$A$12:$F$12</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -244,15 +255,17 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color indexed="12"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -266,11 +279,6 @@
     </fill>
     <fill>
       <patternFill patternType="none">
-        <fgColor rgb="FF1E5885"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF1E5885"/>
       </patternFill>
     </fill>
@@ -302,7 +310,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -313,8 +321,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -347,7 +353,7 @@
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1170927</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:row>0</xdr:row>
       <xdr:rowOff>3810</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -396,7 +402,7 @@
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1504383</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:row>0</xdr:row>
       <xdr:rowOff>3810</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -733,10 +739,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -747,109 +753,98 @@
     <col min="4" max="4" width="45" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="43.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="4"/>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-    </row>
-    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B9" s="2" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B8" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="48" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+      <c r="B13" s="3"/>
+    </row>
+    <row r="14" spans="1:2" ht="80" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" s="3"/>
-    </row>
-    <row r="15" spans="1:6" ht="80" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B14" s="3" t="s">
         <v>21</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:F1"/>
-  </mergeCells>
   <printOptions horizontalCentered="1" gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape"/>
@@ -862,11 +857,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="13" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G34" sqref="G34"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="12" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -879,109 +874,124 @@
     <col min="7" max="7" width="9.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="43.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="4"/>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-    </row>
-    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B9" s="2" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B8" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
+      <c r="A12" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B12" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="G12" s="1" t="s">
         <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>3</v>
@@ -996,15 +1006,15 @@
         <v>34</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>3</v>
@@ -1019,15 +1029,15 @@
         <v>34</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>3</v>
@@ -1041,16 +1051,16 @@
       <c r="F16" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="G16" s="3" t="s">
-        <v>58</v>
+      <c r="G16" s="4" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>3</v>
@@ -1064,16 +1074,16 @@
       <c r="F17" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="G17" s="6" t="s">
-        <v>59</v>
+      <c r="G17" s="4" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>3</v>
@@ -1087,16 +1097,16 @@
       <c r="F18" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="G18" s="6" t="s">
-        <v>60</v>
+      <c r="G18" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>3</v>
@@ -1111,15 +1121,15 @@
         <v>34</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>3</v>
@@ -1134,15 +1144,15 @@
         <v>34</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>3</v>
@@ -1157,15 +1167,15 @@
         <v>34</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>3</v>
@@ -1180,15 +1190,15 @@
         <v>34</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>3</v>
@@ -1203,37 +1213,11 @@
         <v>34</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="G24" s="3" t="s">
         <v>66</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A13:F13" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
-  <mergeCells count="1">
-    <mergeCell ref="A1:F1"/>
-  </mergeCells>
+  <autoFilter ref="A12:F12" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <printOptions horizontalCentered="1" gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape"/>

</xml_diff>